<commit_message>
Koordinaten gesnappt und reale Distanzen berechnet
</commit_message>
<xml_diff>
--- a/Data/sfd-initial-values.xlsx
+++ b/Data/sfd-initial-values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annel\Documents\Locating-APLs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD84AC5-775F-45A1-B241-8971A30874E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28886C70-4C69-4631-BBB0-1E2DCABFB711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{69B7EAA4-B6DB-4D41-AFFE-4C39C5E45C34}"/>
   </bookViews>
@@ -238,22 +238,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -606,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48A7C597-F169-432C-9CE1-7B3758EAC746}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,7 +623,7 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -643,13 +635,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="9">
         <v>131316</v>
       </c>
-      <c r="E2" s="4"/>
       <c r="F2" t="s">
         <v>11</v>
       </c>
@@ -659,13 +650,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -673,39 +664,37 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="9">
+      <c r="C6" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <v>0.63</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -713,161 +702,151 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="9">
+      <c r="C10" s="5">
         <v>0.15</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="8">
         <v>0.19</v>
       </c>
-      <c r="E10" s="4"/>
       <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>5</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <v>5</v>
       </c>
-      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" s="3"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="7">
+      <c r="B20" s="3"/>
+      <c r="C20" s="4">
         <v>6000</v>
       </c>
-      <c r="D20" s="7">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="D20" s="4">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -875,37 +854,37 @@
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
       <c r="E23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="7">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4">
         <v>5500</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="4">
         <v>5500</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="7">
+      <c r="B25" s="3"/>
+      <c r="C25" s="4">
         <v>72000</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>72000</v>
       </c>
       <c r="E25" t="s">
@@ -913,21 +892,21 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="9">
+      <c r="B26" s="3"/>
+      <c r="C26" s="5">
         <v>0.4</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="5">
         <v>0.4</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>